<commit_message>
multi segment 3 changes
</commit_message>
<xml_diff>
--- a/cypress/fixtures/flightDetails.xlsx
+++ b/cypress/fixtures/flightDetails.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="93">
   <si>
     <t>LHR</t>
   </si>
@@ -286,6 +286,30 @@
   </si>
   <si>
     <t>OW</t>
+  </si>
+  <si>
+    <t>Cabin Class 2</t>
+  </si>
+  <si>
+    <t>Departure Location 2</t>
+  </si>
+  <si>
+    <t>Return Location 2</t>
+  </si>
+  <si>
+    <t>Departure Date 2</t>
+  </si>
+  <si>
+    <t>Departure Location 3</t>
+  </si>
+  <si>
+    <t>Return Location 3</t>
+  </si>
+  <si>
+    <t>Departure Date 3</t>
+  </si>
+  <si>
+    <t>Cabin Class 3</t>
   </si>
 </sst>
 </file>
@@ -682,66 +706,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5234375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="4" max="4" width="19.5234375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.5234375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.5234375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="19.5234375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -749,81 +770,77 @@
         <v>15</v>
       </c>
       <c r="C2" s="7">
-        <v>45515</v>
-      </c>
-      <c r="D2" s="7">
-        <v>45454</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>45637</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
       <c r="G2" s="2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2">
         <v>1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>2</v>
       </c>
       <c r="I2" s="2">
         <v>1</v>
       </c>
-      <c r="J2" s="2">
-        <v>1</v>
+      <c r="J2" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="K2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="L2" s="2" t="b">
+      <c r="M2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="N2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="7">
+      <c r="C3" s="7">
         <v>45484</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
       <c r="G3" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I3" s="2">
         <v>0</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="L3" s="2" t="b">
+      <c r="M3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="N3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="N3" t="s">
         <v>84</v>
       </c>
     </row>
@@ -949,18 +966,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="17" max="17" width="10.7890625" customWidth="1"/>
+    <col min="3" max="3" width="11.89453125" customWidth="1"/>
+    <col min="16" max="16" width="11.89453125" customWidth="1"/>
+    <col min="20" max="20" width="11.89453125" customWidth="1"/>
+    <col min="22" max="22" width="16.5234375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:22" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -971,76 +991,64 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+        <v>92</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1050,74 +1058,67 @@
       <c r="C2" s="10">
         <v>45602</v>
       </c>
-      <c r="D2" s="10">
-        <v>45606</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>56</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="K2" s="2" t="b">
-        <v>0</v>
+      <c r="K2" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" s="10">
-        <v>45602</v>
+      <c r="P2" s="10">
+        <v>45609</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" s="10">
-        <v>45606</v>
-      </c>
-      <c r="V2" s="2" t="s">
+      <c r="T2" s="10">
+        <v>45611</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y2" s="10">
-        <v>45609</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>56</v>
+      <c r="V2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="V3" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>